<commit_message>
figures Meta model and meta regression
</commit_message>
<xml_diff>
--- a/data/meta_regression/ph/out3_est_wi.xlsx
+++ b/data/meta_regression/ph/out3_est_wi.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t xml:space="preserve">var</t>
   </si>
@@ -156,9 +156,6 @@
   </si>
   <si>
     <t xml:space="preserve">others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tubers</t>
   </si>
   <si>
     <t xml:space="preserve">vegetable</t>
@@ -545,16 +542,16 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>0.312</v>
+        <v>0.297</v>
       </c>
       <c r="D2" t="n">
-        <v>0.044</v>
+        <v>0.072</v>
       </c>
       <c r="E2" t="n">
-        <v>0.226</v>
+        <v>0.157</v>
       </c>
       <c r="F2" t="n">
-        <v>0.398</v>
+        <v>0.438</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -568,19 +565,19 @@
         <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>0.005</v>
+        <v>-0.055</v>
       </c>
       <c r="D3" t="n">
-        <v>0.039</v>
+        <v>0.045</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.07</v>
+        <v>-0.144</v>
       </c>
       <c r="F3" t="n">
-        <v>0.081</v>
+        <v>0.034</v>
       </c>
       <c r="G3" t="n">
-        <v>0.889</v>
+        <v>0.222</v>
       </c>
     </row>
     <row r="4">
@@ -591,16 +588,16 @@
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>1.014</v>
+        <v>1.154</v>
       </c>
       <c r="D4" t="n">
-        <v>0.179</v>
+        <v>0.206</v>
       </c>
       <c r="E4" t="n">
-        <v>0.663</v>
+        <v>0.75</v>
       </c>
       <c r="F4" t="n">
-        <v>1.366</v>
+        <v>1.559</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -614,16 +611,16 @@
         <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>0.566</v>
+        <v>1.088</v>
       </c>
       <c r="D5" t="n">
-        <v>0.088</v>
+        <v>0.234</v>
       </c>
       <c r="E5" t="n">
-        <v>0.393</v>
+        <v>0.628</v>
       </c>
       <c r="F5" t="n">
-        <v>0.739</v>
+        <v>1.547</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -637,19 +634,19 @@
         <v>13</v>
       </c>
       <c r="C6" t="n">
-        <v>0.27</v>
+        <v>0.661</v>
       </c>
       <c r="D6" t="n">
-        <v>0.095</v>
+        <v>0.154</v>
       </c>
       <c r="E6" t="n">
-        <v>0.084</v>
+        <v>0.359</v>
       </c>
       <c r="F6" t="n">
-        <v>0.456</v>
+        <v>0.963</v>
       </c>
       <c r="G6" t="n">
-        <v>0.004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -663,16 +660,16 @@
         <v>0.693</v>
       </c>
       <c r="D7" t="n">
-        <v>0.594</v>
+        <v>0.643</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.472</v>
+        <v>-0.567</v>
       </c>
       <c r="F7" t="n">
-        <v>1.858</v>
+        <v>1.954</v>
       </c>
       <c r="G7" t="n">
-        <v>0.244</v>
+        <v>0.281</v>
       </c>
     </row>
     <row r="8">
@@ -683,16 +680,16 @@
         <v>15</v>
       </c>
       <c r="C8" t="n">
-        <v>1.436</v>
+        <v>1.874</v>
       </c>
       <c r="D8" t="n">
-        <v>0.27</v>
+        <v>0.324</v>
       </c>
       <c r="E8" t="n">
-        <v>0.907</v>
+        <v>1.238</v>
       </c>
       <c r="F8" t="n">
-        <v>1.965</v>
+        <v>2.509</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -706,19 +703,19 @@
         <v>16</v>
       </c>
       <c r="C9" t="n">
-        <v>0.356</v>
+        <v>0.349</v>
       </c>
       <c r="D9" t="n">
-        <v>0.143</v>
+        <v>0.186</v>
       </c>
       <c r="E9" t="n">
-        <v>0.075</v>
+        <v>-0.015</v>
       </c>
       <c r="F9" t="n">
-        <v>0.637</v>
+        <v>0.713</v>
       </c>
       <c r="G9" t="n">
-        <v>0.013</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="10">
@@ -729,19 +726,19 @@
         <v>17</v>
       </c>
       <c r="C10" t="n">
-        <v>0.758</v>
+        <v>0.125</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1</v>
+        <v>0.387</v>
       </c>
       <c r="E10" t="n">
-        <v>0.561</v>
+        <v>-0.634</v>
       </c>
       <c r="F10" t="n">
-        <v>0.954</v>
+        <v>0.884</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.747</v>
       </c>
     </row>
     <row r="11">
@@ -752,19 +749,19 @@
         <v>18</v>
       </c>
       <c r="C11" t="n">
-        <v>0.466</v>
+        <v>1.222</v>
       </c>
       <c r="D11" t="n">
-        <v>0.141</v>
+        <v>0.246</v>
       </c>
       <c r="E11" t="n">
-        <v>0.189</v>
+        <v>0.74</v>
       </c>
       <c r="F11" t="n">
-        <v>0.742</v>
+        <v>1.705</v>
       </c>
       <c r="G11" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -775,19 +772,19 @@
         <v>19</v>
       </c>
       <c r="C12" t="n">
-        <v>0.061</v>
+        <v>1.111</v>
       </c>
       <c r="D12" t="n">
-        <v>0.145</v>
+        <v>0.302</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.223</v>
+        <v>0.519</v>
       </c>
       <c r="F12" t="n">
-        <v>0.345</v>
+        <v>1.703</v>
       </c>
       <c r="G12" t="n">
-        <v>0.675</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -798,16 +795,16 @@
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>0.199</v>
+        <v>0.302</v>
       </c>
       <c r="D13" t="n">
-        <v>0.042</v>
+        <v>0.059</v>
       </c>
       <c r="E13" t="n">
-        <v>0.118</v>
+        <v>0.186</v>
       </c>
       <c r="F13" t="n">
-        <v>0.281</v>
+        <v>0.418</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -821,19 +818,19 @@
         <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.089</v>
+        <v>-0.185</v>
       </c>
       <c r="D14" t="n">
-        <v>0.04</v>
+        <v>0.066</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.167</v>
+        <v>-0.315</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.01</v>
+        <v>-0.055</v>
       </c>
       <c r="G14" t="n">
-        <v>0.027</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="15">
@@ -847,16 +844,16 @@
         <v>0.051</v>
       </c>
       <c r="D15" t="n">
-        <v>0.475</v>
+        <v>0.545</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.88</v>
+        <v>-1.018</v>
       </c>
       <c r="F15" t="n">
-        <v>0.982</v>
+        <v>1.12</v>
       </c>
       <c r="G15" t="n">
-        <v>0.915</v>
+        <v>0.926</v>
       </c>
     </row>
     <row r="16">
@@ -867,19 +864,19 @@
         <v>24</v>
       </c>
       <c r="C16" t="n">
-        <v>0.467</v>
+        <v>0.479</v>
       </c>
       <c r="D16" t="n">
-        <v>0.226</v>
+        <v>0.255</v>
       </c>
       <c r="E16" t="n">
-        <v>0.024</v>
+        <v>-0.021</v>
       </c>
       <c r="F16" t="n">
-        <v>0.909</v>
+        <v>0.978</v>
       </c>
       <c r="G16" t="n">
-        <v>0.039</v>
+        <v>0.061</v>
       </c>
     </row>
     <row r="17">
@@ -890,16 +887,16 @@
         <v>25</v>
       </c>
       <c r="C17" t="n">
-        <v>0.521</v>
+        <v>0.96</v>
       </c>
       <c r="D17" t="n">
-        <v>0.044</v>
+        <v>0.09</v>
       </c>
       <c r="E17" t="n">
-        <v>0.435</v>
+        <v>0.784</v>
       </c>
       <c r="F17" t="n">
-        <v>0.608</v>
+        <v>1.136</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -913,19 +910,19 @@
         <v>8</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.181</v>
+        <v>-0.057</v>
       </c>
       <c r="D18" t="n">
-        <v>0.045</v>
+        <v>0.103</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.269</v>
+        <v>-0.259</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.094</v>
+        <v>0.145</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>0.582</v>
       </c>
     </row>
     <row r="19">
@@ -936,16 +933,16 @@
         <v>8</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.3</v>
+        <v>-0.344</v>
       </c>
       <c r="D19" t="n">
-        <v>0.045</v>
+        <v>0.087</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.388</v>
+        <v>-0.515</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.212</v>
+        <v>-0.173</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
@@ -959,19 +956,19 @@
         <v>8</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.021</v>
+        <v>-0.05</v>
       </c>
       <c r="D20" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-0.14</v>
+      </c>
+      <c r="F20" t="n">
         <v>0.04</v>
       </c>
-      <c r="E20" t="n">
-        <v>-0.099</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.057</v>
-      </c>
       <c r="G20" t="n">
-        <v>0.601</v>
+        <v>0.274</v>
       </c>
     </row>
     <row r="21">
@@ -982,19 +979,19 @@
         <v>8</v>
       </c>
       <c r="C21" t="n">
-        <v>0.38</v>
+        <v>0.483</v>
       </c>
       <c r="D21" t="n">
-        <v>0.111</v>
+        <v>0.121</v>
       </c>
       <c r="E21" t="n">
-        <v>0.162</v>
+        <v>0.246</v>
       </c>
       <c r="F21" t="n">
-        <v>0.598</v>
+        <v>0.719</v>
       </c>
       <c r="G21" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1008,16 +1005,16 @@
         <v>0.241</v>
       </c>
       <c r="D22" t="n">
-        <v>0.237</v>
+        <v>0.242</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.224</v>
+        <v>-0.234</v>
       </c>
       <c r="F22" t="n">
-        <v>0.705</v>
+        <v>0.715</v>
       </c>
       <c r="G22" t="n">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="23">
@@ -1028,16 +1025,16 @@
         <v>32</v>
       </c>
       <c r="C23" t="n">
-        <v>0.843</v>
+        <v>0.853</v>
       </c>
       <c r="D23" t="n">
-        <v>0.208</v>
+        <v>0.212</v>
       </c>
       <c r="E23" t="n">
-        <v>0.434</v>
+        <v>0.437</v>
       </c>
       <c r="F23" t="n">
-        <v>1.251</v>
+        <v>1.269</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -1054,16 +1051,16 @@
         <v>0.051</v>
       </c>
       <c r="D24" t="n">
-        <v>0.475</v>
+        <v>0.485</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.88</v>
+        <v>-0.9</v>
       </c>
       <c r="F24" t="n">
-        <v>0.982</v>
+        <v>1.002</v>
       </c>
       <c r="G24" t="n">
-        <v>0.915</v>
+        <v>0.916</v>
       </c>
     </row>
     <row r="25">
@@ -1074,19 +1071,19 @@
         <v>34</v>
       </c>
       <c r="C25" t="n">
-        <v>0.557</v>
+        <v>0.558</v>
       </c>
       <c r="D25" t="n">
-        <v>0.342</v>
+        <v>0.348</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.112</v>
+        <v>-0.125</v>
       </c>
       <c r="F25" t="n">
-        <v>1.227</v>
+        <v>1.241</v>
       </c>
       <c r="G25" t="n">
-        <v>0.103</v>
+        <v>0.109</v>
       </c>
     </row>
     <row r="26">
@@ -1100,16 +1097,16 @@
         <v>0.277</v>
       </c>
       <c r="D26" t="n">
-        <v>0.474</v>
+        <v>0.484</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.651</v>
+        <v>-0.671</v>
       </c>
       <c r="F26" t="n">
-        <v>1.205</v>
+        <v>1.225</v>
       </c>
       <c r="G26" t="n">
-        <v>0.559</v>
+        <v>0.567</v>
       </c>
     </row>
     <row r="27">
@@ -1120,16 +1117,16 @@
         <v>36</v>
       </c>
       <c r="C27" t="n">
-        <v>0.771</v>
+        <v>0.778</v>
       </c>
       <c r="D27" t="n">
-        <v>0.14</v>
+        <v>0.143</v>
       </c>
       <c r="E27" t="n">
-        <v>0.497</v>
+        <v>0.498</v>
       </c>
       <c r="F27" t="n">
-        <v>1.046</v>
+        <v>1.058</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
@@ -1143,16 +1140,16 @@
         <v>37</v>
       </c>
       <c r="C28" t="n">
-        <v>1.277</v>
+        <v>1.278</v>
       </c>
       <c r="D28" t="n">
-        <v>0.45</v>
+        <v>0.458</v>
       </c>
       <c r="E28" t="n">
-        <v>0.395</v>
+        <v>0.381</v>
       </c>
       <c r="F28" t="n">
-        <v>2.16</v>
+        <v>2.176</v>
       </c>
       <c r="G28" t="n">
         <v>0.005</v>
@@ -1166,19 +1163,19 @@
         <v>38</v>
       </c>
       <c r="C29" t="n">
-        <v>0.693</v>
+        <v>0.697</v>
       </c>
       <c r="D29" t="n">
-        <v>0.388</v>
+        <v>0.395</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.067</v>
+        <v>-0.078</v>
       </c>
       <c r="F29" t="n">
-        <v>1.453</v>
+        <v>1.472</v>
       </c>
       <c r="G29" t="n">
-        <v>0.074</v>
+        <v>0.078</v>
       </c>
     </row>
     <row r="30">
@@ -1189,16 +1186,16 @@
         <v>39</v>
       </c>
       <c r="C30" t="n">
-        <v>3.333</v>
+        <v>3.337</v>
       </c>
       <c r="D30" t="n">
-        <v>0.644</v>
+        <v>0.65</v>
       </c>
       <c r="E30" t="n">
-        <v>2.072</v>
+        <v>2.064</v>
       </c>
       <c r="F30" t="n">
-        <v>4.595</v>
+        <v>4.61</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
@@ -1212,16 +1209,16 @@
         <v>40</v>
       </c>
       <c r="C31" t="n">
-        <v>1.021</v>
+        <v>1.03</v>
       </c>
       <c r="D31" t="n">
-        <v>0.14</v>
+        <v>0.143</v>
       </c>
       <c r="E31" t="n">
-        <v>0.746</v>
+        <v>0.749</v>
       </c>
       <c r="F31" t="n">
-        <v>1.295</v>
+        <v>1.31</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
@@ -1235,16 +1232,16 @@
         <v>41</v>
       </c>
       <c r="C32" t="n">
-        <v>3.128</v>
+        <v>3.132</v>
       </c>
       <c r="D32" t="n">
-        <v>0.62</v>
+        <v>0.626</v>
       </c>
       <c r="E32" t="n">
-        <v>1.913</v>
+        <v>1.904</v>
       </c>
       <c r="F32" t="n">
-        <v>4.344</v>
+        <v>4.36</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
@@ -1255,45 +1252,45 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C33" t="n">
-        <v>0.346</v>
+        <v>0.743</v>
       </c>
       <c r="D33" t="n">
-        <v>0.054</v>
+        <v>0.354</v>
       </c>
       <c r="E33" t="n">
-        <v>0.241</v>
+        <v>0.05</v>
       </c>
       <c r="F33" t="n">
-        <v>0.451</v>
+        <v>1.437</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>0.036</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C34" t="n">
-        <v>0.734</v>
+        <v>0.241</v>
       </c>
       <c r="D34" t="n">
-        <v>0.347</v>
+        <v>0.275</v>
       </c>
       <c r="E34" t="n">
-        <v>0.053</v>
+        <v>-0.298</v>
       </c>
       <c r="F34" t="n">
-        <v>1.415</v>
+        <v>0.78</v>
       </c>
       <c r="G34" t="n">
-        <v>0.035</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="35">
@@ -1301,22 +1298,22 @@
         <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C35" t="n">
-        <v>0.241</v>
+        <v>0.94</v>
       </c>
       <c r="D35" t="n">
-        <v>0.237</v>
+        <v>0.109</v>
       </c>
       <c r="E35" t="n">
-        <v>-0.224</v>
+        <v>0.726</v>
       </c>
       <c r="F35" t="n">
-        <v>0.705</v>
+        <v>1.155</v>
       </c>
       <c r="G35" t="n">
-        <v>0.31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1324,19 +1321,19 @@
         <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C36" t="n">
-        <v>0.356</v>
+        <v>0.934</v>
       </c>
       <c r="D36" t="n">
-        <v>0.06</v>
+        <v>0.194</v>
       </c>
       <c r="E36" t="n">
-        <v>0.238</v>
+        <v>0.553</v>
       </c>
       <c r="F36" t="n">
-        <v>0.475</v>
+        <v>1.314</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
@@ -1347,22 +1344,22 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C37" t="n">
-        <v>0.534</v>
+        <v>0.56</v>
       </c>
       <c r="D37" t="n">
-        <v>0.101</v>
+        <v>0.394</v>
       </c>
       <c r="E37" t="n">
-        <v>0.336</v>
+        <v>-0.213</v>
       </c>
       <c r="F37" t="n">
-        <v>0.733</v>
+        <v>1.333</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>0.155</v>
       </c>
     </row>
     <row r="38">
@@ -1370,252 +1367,183 @@
         <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C38" t="n">
-        <v>0.557</v>
+        <v>1.388</v>
       </c>
       <c r="D38" t="n">
-        <v>0.342</v>
+        <v>0.302</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.112</v>
+        <v>0.796</v>
       </c>
       <c r="F38" t="n">
-        <v>1.227</v>
+        <v>1.981</v>
       </c>
       <c r="G38" t="n">
-        <v>0.103</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="C39" t="n">
-        <v>1.039</v>
+        <v>-0.165</v>
       </c>
       <c r="D39" t="n">
-        <v>0.107</v>
+        <v>0.073</v>
       </c>
       <c r="E39" t="n">
-        <v>0.829</v>
+        <v>-0.308</v>
       </c>
       <c r="F39" t="n">
-        <v>1.25</v>
+        <v>-0.022</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C40" t="n">
-        <v>0.275</v>
+        <v>0.014</v>
       </c>
       <c r="D40" t="n">
-        <v>0.271</v>
+        <v>0.044</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.258</v>
+        <v>-0.073</v>
       </c>
       <c r="F40" t="n">
-        <v>0.807</v>
+        <v>0.101</v>
       </c>
       <c r="G40" t="n">
-        <v>0.312</v>
+        <v>0.754</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="C41" t="n">
-        <v>0.637</v>
+        <v>-0.081</v>
       </c>
       <c r="D41" t="n">
-        <v>0.168</v>
+        <v>0.042</v>
       </c>
       <c r="E41" t="n">
-        <v>0.308</v>
+        <v>-0.163</v>
       </c>
       <c r="F41" t="n">
-        <v>0.966</v>
+        <v>0.001</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>0.053</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.007</v>
+        <v>-0.172</v>
       </c>
       <c r="D42" t="n">
-        <v>0.041</v>
+        <v>0.056</v>
       </c>
       <c r="E42" t="n">
-        <v>-0.088</v>
+        <v>-0.282</v>
       </c>
       <c r="F42" t="n">
-        <v>0.074</v>
+        <v>-0.061</v>
       </c>
       <c r="G42" t="n">
-        <v>0.865</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
       </c>
       <c r="C43" t="n">
-        <v>0.037</v>
+        <v>-0.08</v>
       </c>
       <c r="D43" t="n">
-        <v>0.039</v>
+        <v>0.041</v>
       </c>
       <c r="E43" t="n">
-        <v>-0.04</v>
+        <v>-0.16</v>
       </c>
       <c r="F43" t="n">
-        <v>0.114</v>
+        <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>0.343</v>
+        <v>0.049</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.075</v>
+        <v>-0.048</v>
       </c>
       <c r="D44" t="n">
-        <v>0.037</v>
+        <v>0.042</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.148</v>
+        <v>-0.131</v>
       </c>
       <c r="F44" t="n">
-        <v>-0.002</v>
+        <v>0.035</v>
       </c>
       <c r="G44" t="n">
-        <v>0.045</v>
+        <v>0.258</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.232</v>
+        <v>-0.021</v>
       </c>
       <c r="D45" t="n">
-        <v>0.051</v>
+        <v>0.139</v>
       </c>
       <c r="E45" t="n">
-        <v>-0.332</v>
+        <v>-0.294</v>
       </c>
       <c r="F45" t="n">
-        <v>-0.132</v>
+        <v>0.253</v>
       </c>
       <c r="G45" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" t="n">
-        <v>-0.044</v>
-      </c>
-      <c r="D46" t="n">
-        <v>0.036</v>
-      </c>
-      <c r="E46" t="n">
-        <v>-0.114</v>
-      </c>
-      <c r="F46" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0.212</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" t="n">
-        <v>-0.054</v>
-      </c>
-      <c r="D47" t="n">
-        <v>0.037</v>
-      </c>
-      <c r="E47" t="n">
-        <v>-0.127</v>
-      </c>
-      <c r="F47" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="G47" t="n">
-        <v>0.153</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>56</v>
-      </c>
-      <c r="B48" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" t="n">
-        <v>0.094</v>
-      </c>
-      <c r="D48" t="n">
-        <v>0.045</v>
-      </c>
-      <c r="E48" t="n">
-        <v>0.006</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0.183</v>
-      </c>
-      <c r="G48" t="n">
-        <v>0.037</v>
+        <v>0.882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>